<commit_message>
reports on other periods
</commit_message>
<xml_diff>
--- a/Outputs/meanBehavior.xlsx
+++ b/Outputs/meanBehavior.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>REER=100</t>
   </si>
@@ -25,7 +25,10 @@
     <t>REER=EAEU extended (mean)</t>
   </si>
   <si>
-    <t>QADF significance (10%)</t>
+    <t>Mean Reversion (Entire period)</t>
+  </si>
+  <si>
+    <t>Mean Reversion (EAEU only)</t>
   </si>
   <si>
     <t>Countries</t>
@@ -71,6 +74,12 @@
   </si>
   <si>
     <t>0.4-0.9</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.2-0.7</t>
   </si>
 </sst>
 </file>
@@ -456,15 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -478,10 +487,13 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>0.9499999999999995</v>
@@ -493,12 +505,15 @@
         <v>0.3399999999999999</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>0.5699999999999997</v>
@@ -510,12 +525,15 @@
         <v>0.4599999999999999</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0.8299999999999996</v>
@@ -527,12 +545,15 @@
         <v>0.5299999999999998</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>0.5599999999999997</v>
@@ -544,12 +565,15 @@
         <v>0.4199999999999998</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>0.3899999999999999</v>
@@ -561,12 +585,15 @@
         <v>0.4099999999999998</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>0.7299999999999996</v>
@@ -578,12 +605,15 @@
         <v>0.4699999999999999</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0.4899999999999998</v>
@@ -595,12 +625,15 @@
         <v>0.4699999999999999</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>0.9499999999999995</v>
@@ -612,7 +645,10 @@
         <v>0.4099999999999998</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -621,17 +657,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:E1">
+  <conditionalFormatting sqref="A1:F1">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:E9">
+  <conditionalFormatting sqref="A1:F9">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:E9">
+  <conditionalFormatting sqref="A9:F9">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
setar changes will be next
</commit_message>
<xml_diff>
--- a/Outputs/meanBehavior.xlsx
+++ b/Outputs/meanBehavior.xlsx
@@ -14,21 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>REER=100</t>
   </si>
   <si>
-    <t>REER=Before EAEU (mean)</t>
-  </si>
-  <si>
-    <t>REER=EAEU extended (mean)</t>
-  </si>
-  <si>
-    <t>Mean Reversion (Entire period)</t>
-  </si>
-  <si>
-    <t>Mean Reversion (EAEU only)</t>
+    <t>REER=Mean (entire period)</t>
+  </si>
+  <si>
+    <t>REER=Mean (before EAEU)</t>
+  </si>
+  <si>
+    <t>REER=Mean (after EAEU)</t>
+  </si>
+  <si>
+    <t>Mean Reversion (before EAEU)</t>
+  </si>
+  <si>
+    <t>Mean Reversion (after EAEU)</t>
+  </si>
+  <si>
+    <t>Mean Reversion (entire period)</t>
   </si>
   <si>
     <t>Countries</t>
@@ -61,25 +67,43 @@
     <t>N/A</t>
   </si>
   <si>
+    <t>0.5-0.9*</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.6, 0.8</t>
+  </si>
+  <si>
+    <t>0.1-0.4*</t>
+  </si>
+  <si>
+    <t>0.4-0.7*</t>
+  </si>
+  <si>
+    <t>0.7,0.8*</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.2-0.7</t>
+  </si>
+  <si>
     <t>0.1,0.5</t>
   </si>
   <si>
     <t>0.7,0.8</t>
   </si>
   <si>
-    <t>0.5-0.9</t>
-  </si>
-  <si>
     <t>0.1-0.4</t>
   </si>
   <si>
-    <t>0.4-0.9</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>0.2-0.7</t>
+    <t>0.4-0.9*</t>
   </si>
 </sst>
 </file>
@@ -465,15 +489,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -490,165 +514,219 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>0.9499999999999995</v>
       </c>
       <c r="C2">
+        <v>0.3399999999999999</v>
+      </c>
+      <c r="D2">
         <v>0.3199999999999999</v>
       </c>
-      <c r="D2">
-        <v>0.3399999999999999</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
+      <c r="E2">
+        <v>0.7299999999999996</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>0.5699999999999997</v>
       </c>
       <c r="C3">
+        <v>0.4599999999999999</v>
+      </c>
+      <c r="D3">
         <v>0.5699999999999997</v>
       </c>
-      <c r="D3">
-        <v>0.4599999999999999</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
+      <c r="E3">
+        <v>0.1899999999999999</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>0.8299999999999996</v>
       </c>
       <c r="C4">
+        <v>0.5299999999999998</v>
+      </c>
+      <c r="D4">
         <v>0.5799999999999997</v>
       </c>
-      <c r="D4">
-        <v>0.5299999999999998</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+      <c r="E4">
+        <v>0.2499999999999999</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0.5599999999999997</v>
       </c>
       <c r="C5">
+        <v>0.4199999999999998</v>
+      </c>
+      <c r="D5">
         <v>0.3899999999999999</v>
       </c>
-      <c r="D5">
-        <v>0.4199999999999998</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
+      <c r="E5">
+        <v>0.6599999999999997</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>0.3899999999999999</v>
       </c>
       <c r="C6">
+        <v>0.4099999999999998</v>
+      </c>
+      <c r="D6">
         <v>0.3599999999999999</v>
       </c>
-      <c r="D6">
-        <v>0.4099999999999998</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
+      <c r="E6">
+        <v>0.8199999999999996</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>0.7299999999999996</v>
       </c>
       <c r="C7">
+        <v>0.4699999999999999</v>
+      </c>
+      <c r="D7">
         <v>0.4799999999999998</v>
       </c>
-      <c r="D7">
-        <v>0.4699999999999999</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="E7">
+        <v>0.4099999999999998</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>0.4899999999999998</v>
       </c>
       <c r="C8">
+        <v>0.4699999999999999</v>
+      </c>
+      <c r="D8">
         <v>0.6799999999999997</v>
       </c>
-      <c r="D8">
-        <v>0.4699999999999999</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
+      <c r="E8">
+        <v>0.18</v>
       </c>
       <c r="F8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>0.9499999999999995</v>
       </c>
       <c r="C9">
+        <v>0.4099999999999998</v>
+      </c>
+      <c r="D9">
         <v>0.6199999999999998</v>
       </c>
-      <c r="D9">
-        <v>0.4099999999999998</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
+      <c r="E9">
+        <v>0.2</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -657,17 +735,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:F1">
+  <conditionalFormatting sqref="A1:H1">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:F9">
+  <conditionalFormatting sqref="A1:H9">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:F9">
+  <conditionalFormatting sqref="A9:H9">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
       <formula>0</formula>
     </cfRule>

</xml_diff>